<commit_message>
Commit correção cap 14 15/11/2023
</commit_message>
<xml_diff>
--- a/Arquivos/dadosAutoestima2.xlsx
+++ b/Arquivos/dadosAutoestima2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\petro\Dropbox\Estatistica\Meus_Livros\Bioestatistica_R\Book\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\petro\Dropbox\Estatistica\Meus_Livros\bookR\Arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC11C084-16BE-419F-AF4C-3389761AF338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9257353-07F9-48D9-A614-5D0312532F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5055" yWindow="1695" windowWidth="14190" windowHeight="12480" xr2:uid="{88C4B767-C263-4334-8BB2-8989CEEA30BC}"/>
+    <workbookView xWindow="13890" yWindow="900" windowWidth="14190" windowHeight="12480" xr2:uid="{88C4B767-C263-4334-8BB2-8989CEEA30BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -117,12 +117,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -446,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7616BB4D-F10B-4D54-ADAD-7FF75EB30E34}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="F1" sqref="F1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,562 +456,472 @@
     <col min="2" max="2" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4">
         <v>25.2</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>25.8</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>26.4</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5">
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4">
         <v>30</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>29.7</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>29.1</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4">
         <v>27.3</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>27.3</v>
       </c>
-      <c r="E4" s="5">
-        <v>27.6</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="E4" s="4">
+        <v>27.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4">
         <v>27.3</v>
       </c>
-      <c r="D5" s="5">
-        <v>27.6</v>
-      </c>
-      <c r="E5" s="5">
+      <c r="D5" s="4">
+        <v>27.6</v>
+      </c>
+      <c r="E5" s="4">
         <v>28.5</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="5">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4">
         <v>22.2</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>22.8</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>21.6</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4">
         <v>22.8</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>22.5</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>22.8</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4">
         <v>27</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>26.1</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>26.1</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="5">
+      <c r="B9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4">
         <v>26.7</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>26.7</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>26.4</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4">
         <v>27.9</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>28.2</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>27.9</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="B11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="4">
         <v>27</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>27.9</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>28.5</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="5">
+      <c r="B12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4">
         <v>27.9</v>
       </c>
-      <c r="D12" s="5">
-        <v>27.6</v>
-      </c>
-      <c r="E12" s="5">
+      <c r="D12" s="4">
+        <v>27.6</v>
+      </c>
+      <c r="E12" s="4">
         <v>27.3</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="5">
+      <c r="B13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4">
         <v>24</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>24</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>23.4</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>1</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="5">
+      <c r="B14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="4">
         <v>24.9</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>23.1</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>20.7</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>2</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="5">
+      <c r="B15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="4">
         <v>29.1</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>28.5</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>26.4</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>3</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="5">
+      <c r="B16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="4">
         <v>27.9</v>
       </c>
-      <c r="D16" s="5">
-        <v>27.6</v>
-      </c>
-      <c r="E16" s="5">
+      <c r="D16" s="4">
+        <v>27.6</v>
+      </c>
+      <c r="E16" s="4">
         <v>26.7</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
         <v>4</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="5">
-        <v>27.6</v>
-      </c>
-      <c r="D17" s="5">
-        <v>27.6</v>
-      </c>
-      <c r="E17" s="5">
+      <c r="B17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="4">
+        <v>27.6</v>
+      </c>
+      <c r="D17" s="4">
+        <v>27.6</v>
+      </c>
+      <c r="E17" s="4">
         <v>26.7</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>5</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="5">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>5</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="4">
         <v>23.1</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>21.9</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <v>20.399999999999999</v>
       </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>6</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="5">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>6</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="4">
         <v>21.6</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>19.5</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>18.899999999999999</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
         <v>7</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="5">
-        <v>27.6</v>
-      </c>
-      <c r="D20" s="5">
+      <c r="B20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="4">
+        <v>27.6</v>
+      </c>
+      <c r="D20" s="4">
         <v>26.7</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <v>23.7</v>
       </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
         <v>8</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="5">
-        <v>27.6</v>
-      </c>
-      <c r="D21" s="5">
+      <c r="B21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="4">
+        <v>27.6</v>
+      </c>
+      <c r="D21" s="4">
         <v>26.1</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="4">
         <v>24.3</v>
       </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
         <v>9</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="5">
+      <c r="B22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="4">
         <v>28.5</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
         <v>27.3</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="4">
         <v>25.2</v>
       </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
         <v>10</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="5">
-        <v>27.6</v>
-      </c>
-      <c r="D23" s="5">
+      <c r="B23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="4">
+        <v>27.6</v>
+      </c>
+      <c r="D23" s="4">
         <v>25.2</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="4">
         <v>24.3</v>
       </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
         <v>11</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="5">
-        <v>27.6</v>
-      </c>
-      <c r="D24" s="5">
-        <v>27.6</v>
-      </c>
-      <c r="E24" s="5">
+      <c r="B24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="4">
+        <v>27.6</v>
+      </c>
+      <c r="D24" s="4">
+        <v>27.6</v>
+      </c>
+      <c r="E24" s="4">
         <v>27.3</v>
       </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
         <v>12</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="5">
+      <c r="B25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="4">
         <v>23.7</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="4">
         <v>20.7</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="4">
         <v>18.600000000000001</v>
       </c>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E25">

</xml_diff>